<commit_message>
feat: Added visualization using matplotlib and a lot of refactoring.
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\PowerAwareIOTProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AB42F7-07EB-47C8-8B16-350FFCB0F2EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5BEAE7-C2C1-49A7-96F4-BA7E0A2D42A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iot_sensor_data" sheetId="1" r:id="rId1"/>
@@ -103,10 +103,10 @@
     <t>Storage</t>
   </si>
   <si>
-    <t>Processsing</t>
+    <t>Humidty</t>
   </si>
   <si>
-    <t>Humidty</t>
+    <t>Data Processsing</t>
   </si>
 </sst>
 </file>
@@ -619,11 +619,11 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -13468,8 +13468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N578"/>
   <sheetViews>
-    <sheetView topLeftCell="A552" workbookViewId="0">
-      <selection sqref="A1:B578"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13653,7 +13653,7 @@
         <v/>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -20474,7 +20474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF2D61A0-1F3D-4051-B8AC-8F112607127D}">
   <dimension ref="C1:L578"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
@@ -20500,7 +20500,7 @@
         <v>1</v>
       </c>
       <c r="L1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="3:12" x14ac:dyDescent="0.25">

</xml_diff>